<commit_message>
Recalculated FOCB and CBEP comparisons using pH Total
Also made table row labels more consistent accross the two data sets.
</commit_message>
<xml_diff>
--- a/Analysis/Monthly_summaries_OA_CBEP_and_FOCB.xlsx
+++ b/Analysis/Monthly_summaries_OA_CBEP_and_FOCB.xlsx
@@ -5,21 +5,27 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Dropbox\Work\CBEP_OA\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\curtis.bohlen\Desktop\Current Projects\State of the Bay 2020\Data\CBEP_OA\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="5030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6760"/>
   </bookViews>
   <sheets>
-    <sheet name="Monthly_summaries_OA_CBEP" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly_summaries_OA_FOCB" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="36">
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
   <si>
     <t>Jan</t>
   </si>
@@ -57,6 +63,9 @@
     <t>Dec</t>
   </si>
   <si>
+    <t>chl</t>
+  </si>
+  <si>
     <t>avg</t>
   </si>
   <si>
@@ -69,40 +78,55 @@
     <t>count</t>
   </si>
   <si>
-    <t>Site</t>
+    <t>do</t>
+  </si>
+  <si>
+    <t>omega_a</t>
+  </si>
+  <si>
+    <t>pco2</t>
+  </si>
+  <si>
+    <t>pco2_corr</t>
+  </si>
+  <si>
+    <t>pctsat</t>
+  </si>
+  <si>
+    <t>ph_tot</t>
+  </si>
+  <si>
+    <t>salinity</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>FOCB</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>co2_corr</t>
+  </si>
+  <si>
+    <t>do_mgpl</t>
+  </si>
+  <si>
+    <t>sal</t>
+  </si>
+  <si>
+    <t>temp</t>
   </si>
   <si>
     <t>CBEP</t>
   </si>
   <si>
-    <t>FOCB</t>
-  </si>
-  <si>
-    <t>Parameter</t>
-  </si>
-  <si>
-    <t>Statistic</t>
-  </si>
-  <si>
-    <t>pCO2</t>
-  </si>
-  <si>
-    <t>pCO2_corr</t>
-  </si>
-  <si>
-    <t>DO</t>
-  </si>
-  <si>
-    <t>Omega_a</t>
-  </si>
-  <si>
-    <t>Salinity</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>pH</t>
+    <t>ph_NSB</t>
   </si>
 </sst>
 </file>
@@ -909,249 +933,244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O57"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" customWidth="1"/>
-    <col min="3" max="3" width="7.1796875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D2">
-        <v>13.34</v>
+        <v>11.72</v>
       </c>
       <c r="E2">
-        <v>13.14</v>
+        <v>7.24</v>
       </c>
       <c r="F2">
-        <v>13.19</v>
+        <v>12.45</v>
       </c>
       <c r="G2">
-        <v>13.21</v>
+        <v>8.65</v>
       </c>
       <c r="H2">
-        <v>12.43</v>
+        <v>3.38</v>
       </c>
       <c r="I2">
-        <v>11.36</v>
+        <v>3.79</v>
       </c>
       <c r="J2">
-        <v>10.9</v>
+        <v>5.27</v>
       </c>
       <c r="K2">
-        <v>10.029999999999999</v>
+        <v>6.87</v>
       </c>
       <c r="L2">
-        <v>9.36</v>
+        <v>7.83</v>
       </c>
       <c r="M2">
-        <v>9.51</v>
+        <v>7.12</v>
       </c>
       <c r="N2">
-        <v>10.32</v>
+        <v>5.75</v>
       </c>
       <c r="O2">
-        <v>11.31</v>
+        <v>9.6300000000000008</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D3">
-        <v>11.85</v>
+        <v>12.41</v>
       </c>
       <c r="E3">
-        <v>12.07</v>
+        <v>5.9</v>
       </c>
       <c r="F3">
-        <v>11.78</v>
+        <v>7.93</v>
       </c>
       <c r="G3">
-        <v>11.36</v>
+        <v>4.26</v>
       </c>
       <c r="H3">
-        <v>10.47</v>
+        <v>2.54</v>
       </c>
       <c r="I3">
-        <v>9.43</v>
+        <v>3.31</v>
       </c>
       <c r="J3">
-        <v>8.9700000000000006</v>
+        <v>4.42</v>
       </c>
       <c r="K3">
-        <v>8.6999999999999993</v>
+        <v>5.65</v>
       </c>
       <c r="L3">
-        <v>8.2100000000000009</v>
+        <v>5.58</v>
       </c>
       <c r="M3">
-        <v>8.33</v>
+        <v>6.06</v>
       </c>
       <c r="N3">
-        <v>9.2799999999999994</v>
+        <v>4.33</v>
       </c>
       <c r="O3">
-        <v>10.69</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>175</v>
+        <v>6.0010000000000003</v>
       </c>
       <c r="E4">
-        <v>534</v>
+        <v>5.6959999999999997</v>
       </c>
       <c r="F4">
-        <v>376</v>
+        <v>14.760999999999999</v>
       </c>
       <c r="G4">
-        <v>687</v>
+        <v>10.516</v>
       </c>
       <c r="H4">
-        <v>2218</v>
+        <v>3.0089999999999999</v>
       </c>
       <c r="I4">
-        <v>2072</v>
+        <v>2.6429999999999998</v>
       </c>
       <c r="J4">
-        <v>1464</v>
+        <v>3.8879999999999999</v>
       </c>
       <c r="K4">
-        <v>2161</v>
+        <v>5.3220000000000001</v>
       </c>
       <c r="L4">
-        <v>2732</v>
+        <v>7.1180000000000003</v>
       </c>
       <c r="M4">
-        <v>2660</v>
+        <v>4.101</v>
       </c>
       <c r="N4">
-        <v>1975</v>
+        <v>4.6539999999999999</v>
       </c>
       <c r="O4">
-        <v>1488</v>
+        <v>9.4730000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>2231</v>
       </c>
       <c r="E5">
-        <v>1803</v>
+        <v>2016</v>
       </c>
       <c r="F5">
-        <v>2214</v>
+        <v>2221</v>
       </c>
       <c r="G5">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="H5">
-        <v>2070</v>
+        <v>2166</v>
       </c>
       <c r="I5">
-        <v>2157</v>
+        <v>2175</v>
       </c>
       <c r="J5">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="K5">
-        <v>2947</v>
+        <v>2942</v>
       </c>
       <c r="L5">
-        <v>2879</v>
+        <v>2802</v>
       </c>
       <c r="M5">
         <v>2975</v>
       </c>
       <c r="N5">
-        <v>2421</v>
+        <v>2430</v>
       </c>
       <c r="O5">
         <v>2964</v>
@@ -1159,60 +1178,60 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D6">
-        <v>13.37</v>
+        <v>11.85</v>
       </c>
       <c r="E6">
-        <v>13.15</v>
+        <v>12.07</v>
       </c>
       <c r="F6">
-        <v>13.2</v>
+        <v>11.78</v>
       </c>
       <c r="G6">
-        <v>13.29</v>
+        <v>11.36</v>
       </c>
       <c r="H6">
-        <v>12.42</v>
+        <v>10.47</v>
       </c>
       <c r="I6">
-        <v>11.41</v>
+        <v>9.43</v>
       </c>
       <c r="J6">
-        <v>10.82</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="K6">
-        <v>10.19</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="L6">
-        <v>9.6</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="M6">
-        <v>9.8699999999999992</v>
+        <v>8.33</v>
       </c>
       <c r="N6">
-        <v>10.35</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="O6">
-        <v>11.13</v>
+        <v>10.69</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D7">
         <v>11.79</v>
@@ -1253,236 +1272,248 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>0.11700000000000001</v>
+        <v>0.63700000000000001</v>
       </c>
       <c r="E8">
-        <v>0.20599999999999999</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="F8">
-        <v>0.16400000000000001</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="G8">
-        <v>0.39300000000000002</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="H8">
-        <v>0.61799999999999999</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="I8">
-        <v>0.67500000000000004</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="J8">
-        <v>0.79800000000000004</v>
+        <v>0.78</v>
       </c>
       <c r="K8">
-        <v>0.89700000000000002</v>
+        <v>0.871</v>
       </c>
       <c r="L8">
-        <v>1.2190000000000001</v>
+        <v>0.83599999999999997</v>
       </c>
       <c r="M8">
-        <v>1.0589999999999999</v>
+        <v>0.624</v>
       </c>
       <c r="N8">
-        <v>0.55700000000000005</v>
+        <v>0.60299999999999998</v>
       </c>
       <c r="O8">
-        <v>0.873</v>
+        <v>0.72599999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>0.63700000000000001</v>
+        <v>2231</v>
       </c>
       <c r="E9">
-        <v>0.67800000000000005</v>
+        <v>1803</v>
       </c>
       <c r="F9">
-        <v>0.63400000000000001</v>
+        <v>2214</v>
       </c>
       <c r="G9">
-        <v>0.69699999999999995</v>
+        <v>2160</v>
       </c>
       <c r="H9">
-        <v>0.65400000000000003</v>
+        <v>2070</v>
       </c>
       <c r="I9">
-        <v>0.74</v>
+        <v>2175</v>
       </c>
       <c r="J9">
-        <v>0.78</v>
+        <v>2504</v>
       </c>
       <c r="K9">
-        <v>0.871</v>
+        <v>2947</v>
       </c>
       <c r="L9">
-        <v>0.83599999999999997</v>
+        <v>2879</v>
       </c>
       <c r="M9">
-        <v>0.624</v>
+        <v>2975</v>
       </c>
       <c r="N9">
-        <v>0.60299999999999998</v>
+        <v>2431</v>
       </c>
       <c r="O9">
-        <v>0.72599999999999998</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
+      </c>
+      <c r="E10">
+        <v>1.08</v>
+      </c>
+      <c r="F10">
+        <v>1.07</v>
       </c>
       <c r="G10">
-        <v>1.91</v>
+        <v>0.78</v>
       </c>
       <c r="H10">
-        <v>1.99</v>
+        <v>0.9</v>
       </c>
       <c r="I10">
-        <v>1.61</v>
+        <v>1.31</v>
       </c>
       <c r="J10">
-        <v>1.76</v>
+        <v>1.56</v>
       </c>
       <c r="K10">
-        <v>1.71</v>
+        <v>1.68</v>
       </c>
       <c r="L10">
-        <v>1.51</v>
+        <v>1.47</v>
       </c>
       <c r="M10">
-        <v>1.64</v>
+        <v>1.38</v>
       </c>
       <c r="N10">
-        <v>0.61</v>
+        <v>0.98</v>
+      </c>
+      <c r="O10">
+        <v>1.01</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D11">
-        <v>0.8</v>
+        <v>0.77</v>
       </c>
       <c r="E11">
-        <v>1.08</v>
+        <v>0.95</v>
       </c>
       <c r="F11">
-        <v>1.07</v>
+        <v>1.05</v>
       </c>
       <c r="G11">
-        <v>0.78</v>
+        <v>0.73</v>
       </c>
       <c r="H11">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="I11">
-        <v>1.31</v>
+        <v>1.2</v>
       </c>
       <c r="J11">
-        <v>1.56</v>
+        <v>1.53</v>
       </c>
       <c r="K11">
-        <v>1.68</v>
+        <v>1.58</v>
       </c>
       <c r="L11">
-        <v>1.47</v>
+        <v>1.43</v>
       </c>
       <c r="M11">
-        <v>1.38</v>
+        <v>1.33</v>
       </c>
       <c r="N11">
         <v>0.98</v>
       </c>
       <c r="O11">
-        <v>1.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.30099999999999999</v>
       </c>
       <c r="G12">
-        <v>174</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="H12">
-        <v>725</v>
+        <v>0.311</v>
       </c>
       <c r="I12">
-        <v>1030</v>
+        <v>0.432</v>
       </c>
       <c r="J12">
-        <v>1322</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="K12">
-        <v>1112</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="L12">
-        <v>1047</v>
+        <v>0.307</v>
       </c>
       <c r="M12">
-        <v>1542</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="N12">
-        <v>158</v>
+        <v>0.21</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>0.17499999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D13">
         <v>835</v>
@@ -1500,7 +1531,7 @@
         <v>1878</v>
       </c>
       <c r="I13">
-        <v>1644</v>
+        <v>1662</v>
       </c>
       <c r="J13">
         <v>1607</v>
@@ -1515,7 +1546,7 @@
         <v>2240</v>
       </c>
       <c r="N13">
-        <v>2093</v>
+        <v>2103</v>
       </c>
       <c r="O13">
         <v>2219</v>
@@ -1523,318 +1554,342 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>27</v>
+      </c>
+      <c r="D14">
+        <v>259.06</v>
+      </c>
+      <c r="E14">
+        <v>280.98</v>
+      </c>
+      <c r="F14">
+        <v>295.27</v>
       </c>
       <c r="G14">
-        <v>1.91</v>
+        <v>367.3</v>
       </c>
       <c r="H14">
-        <v>1.97</v>
+        <v>388.87</v>
       </c>
       <c r="I14">
-        <v>1.67</v>
+        <v>419.36</v>
       </c>
       <c r="J14">
-        <v>1.83</v>
+        <v>526.91999999999996</v>
       </c>
       <c r="K14">
-        <v>1.79</v>
+        <v>510.86</v>
       </c>
       <c r="L14">
-        <v>1.44</v>
+        <v>536.11</v>
       </c>
       <c r="M14">
-        <v>1.61</v>
+        <v>504.17</v>
       </c>
       <c r="N14">
-        <v>0.57999999999999996</v>
+        <v>443.22</v>
+      </c>
+      <c r="O14">
+        <v>350.2</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D15">
-        <v>0.77</v>
+        <v>243.69</v>
       </c>
       <c r="E15">
-        <v>0.95</v>
+        <v>276.88</v>
       </c>
       <c r="F15">
-        <v>1.05</v>
+        <v>318.74</v>
       </c>
       <c r="G15">
-        <v>0.73</v>
+        <v>377.97</v>
       </c>
       <c r="H15">
-        <v>0.93</v>
+        <v>379.81</v>
       </c>
       <c r="I15">
-        <v>1.2</v>
+        <v>415.78</v>
       </c>
       <c r="J15">
-        <v>1.53</v>
+        <v>519.83000000000004</v>
       </c>
       <c r="K15">
-        <v>1.58</v>
+        <v>489.22</v>
       </c>
       <c r="L15">
-        <v>1.43</v>
+        <v>526.72</v>
       </c>
       <c r="M15">
-        <v>1.33</v>
+        <v>503.48</v>
       </c>
       <c r="N15">
-        <v>0.98</v>
+        <v>455.77</v>
       </c>
       <c r="O15">
-        <v>1</v>
+        <v>343.9</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>48.09</v>
+      </c>
+      <c r="E16">
+        <v>40.591000000000001</v>
+      </c>
+      <c r="F16">
+        <v>86.212000000000003</v>
       </c>
       <c r="G16">
-        <v>9.4E-2</v>
+        <v>66.989999999999995</v>
       </c>
       <c r="H16">
-        <v>0.16400000000000001</v>
+        <v>65.465000000000003</v>
       </c>
       <c r="I16">
-        <v>0.36499999999999999</v>
+        <v>55.816000000000003</v>
       </c>
       <c r="J16">
-        <v>0.28999999999999998</v>
+        <v>114.771</v>
       </c>
       <c r="K16">
-        <v>0.54700000000000004</v>
+        <v>99.522999999999996</v>
       </c>
       <c r="L16">
-        <v>0.37</v>
+        <v>80.478999999999999</v>
       </c>
       <c r="M16">
-        <v>0.57999999999999996</v>
+        <v>101.77200000000001</v>
       </c>
       <c r="N16">
-        <v>0.216</v>
+        <v>80.403999999999996</v>
+      </c>
+      <c r="O16">
+        <v>71.730999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D17">
-        <v>0.125</v>
+        <v>835</v>
       </c>
       <c r="E17">
-        <v>0.32900000000000001</v>
+        <v>1349</v>
       </c>
       <c r="F17">
-        <v>0.30099999999999999</v>
+        <v>1734</v>
       </c>
       <c r="G17">
-        <v>0.27300000000000002</v>
+        <v>784</v>
       </c>
       <c r="H17">
-        <v>0.311</v>
+        <v>1878</v>
       </c>
       <c r="I17">
-        <v>0.432</v>
+        <v>1662</v>
       </c>
       <c r="J17">
-        <v>0.41799999999999998</v>
+        <v>1607</v>
       </c>
       <c r="K17">
-        <v>0.57099999999999995</v>
+        <v>1383</v>
       </c>
       <c r="L17">
-        <v>0.307</v>
+        <v>1672</v>
       </c>
       <c r="M17">
-        <v>0.28100000000000003</v>
+        <v>2240</v>
       </c>
       <c r="N17">
-        <v>0.21</v>
+        <v>2103</v>
       </c>
       <c r="O17">
-        <v>0.17499999999999999</v>
+        <v>2219</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D18">
-        <v>376.17</v>
+        <v>413.32</v>
       </c>
       <c r="E18">
-        <v>473.45</v>
+        <v>441.52</v>
       </c>
       <c r="F18">
-        <v>407.76</v>
+        <v>439.51</v>
       </c>
       <c r="G18">
-        <v>301.83999999999997</v>
+        <v>479.7</v>
       </c>
       <c r="H18">
-        <v>398.42</v>
+        <v>422.72</v>
       </c>
       <c r="I18">
-        <v>464.58</v>
+        <v>400.04</v>
       </c>
       <c r="J18">
-        <v>566.19000000000005</v>
+        <v>427.7</v>
       </c>
       <c r="K18">
-        <v>723.6</v>
+        <v>394.84</v>
       </c>
       <c r="L18">
-        <v>736.16</v>
+        <v>443.27</v>
       </c>
       <c r="M18">
-        <v>729.35</v>
+        <v>480.93</v>
       </c>
       <c r="N18">
-        <v>576.75</v>
+        <v>514.51</v>
       </c>
       <c r="O18">
-        <v>491.44</v>
+        <v>489.59</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D19">
-        <v>259.06</v>
+        <v>409.79</v>
       </c>
       <c r="E19">
-        <v>280.98</v>
+        <v>434.3</v>
       </c>
       <c r="F19">
-        <v>295.27</v>
+        <v>454.31</v>
       </c>
       <c r="G19">
-        <v>367.3</v>
+        <v>493.13</v>
       </c>
       <c r="H19">
-        <v>388.87</v>
+        <v>408.93</v>
       </c>
       <c r="I19">
-        <v>419.28</v>
+        <v>396.68</v>
       </c>
       <c r="J19">
-        <v>526.91999999999996</v>
+        <v>419.01</v>
       </c>
       <c r="K19">
-        <v>510.86</v>
+        <v>376.89</v>
       </c>
       <c r="L19">
-        <v>536.11</v>
+        <v>435.25</v>
       </c>
       <c r="M19">
-        <v>504.17</v>
+        <v>492.35</v>
       </c>
       <c r="N19">
-        <v>443.23</v>
+        <v>509.64</v>
       </c>
       <c r="O19">
-        <v>350.2</v>
+        <v>474.45</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D20">
-        <v>735</v>
+        <v>52.307000000000002</v>
       </c>
       <c r="E20">
-        <v>578</v>
+        <v>71.436999999999998</v>
       </c>
       <c r="F20">
-        <v>736</v>
+        <v>130.69900000000001</v>
       </c>
       <c r="G20">
-        <v>639</v>
+        <v>84.088999999999999</v>
       </c>
       <c r="H20">
-        <v>1461</v>
+        <v>80.283000000000001</v>
       </c>
       <c r="I20">
-        <v>1968</v>
+        <v>60.5</v>
       </c>
       <c r="J20">
-        <v>1802</v>
+        <v>98.632999999999996</v>
       </c>
       <c r="K20">
-        <v>2151</v>
+        <v>85.686999999999998</v>
       </c>
       <c r="L20">
-        <v>2699</v>
+        <v>72.546000000000006</v>
       </c>
       <c r="M20">
-        <v>2721</v>
+        <v>90.863</v>
       </c>
       <c r="N20">
-        <v>1575</v>
+        <v>97.275999999999996</v>
       </c>
       <c r="O20">
-        <v>1470</v>
+        <v>90.843999999999994</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D21">
         <v>835</v>
@@ -1852,7 +1907,7 @@
         <v>1878</v>
       </c>
       <c r="I21">
-        <v>1644</v>
+        <v>1662</v>
       </c>
       <c r="J21">
         <v>1607</v>
@@ -1867,7 +1922,7 @@
         <v>2240</v>
       </c>
       <c r="N21">
-        <v>2093</v>
+        <v>2103</v>
       </c>
       <c r="O21">
         <v>2219</v>
@@ -1875,712 +1930,718 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D22">
-        <v>378.6</v>
+        <v>103.41</v>
       </c>
       <c r="E22">
-        <v>464</v>
+        <v>105.61</v>
       </c>
       <c r="F22">
-        <v>431.3</v>
+        <v>106.39</v>
       </c>
       <c r="G22">
-        <v>304.8</v>
+        <v>109.72</v>
       </c>
       <c r="H22">
-        <v>392.4</v>
+        <v>110.57</v>
       </c>
       <c r="I22">
-        <v>467.55</v>
+        <v>108.04</v>
       </c>
       <c r="J22">
-        <v>565.83000000000004</v>
+        <v>111.68</v>
       </c>
       <c r="K22">
-        <v>714.12</v>
+        <v>110.12</v>
       </c>
       <c r="L22">
-        <v>704.93</v>
+        <v>100.85</v>
       </c>
       <c r="M22">
-        <v>707.4</v>
+        <v>96</v>
       </c>
       <c r="N22">
-        <v>562.75</v>
+        <v>95.94</v>
       </c>
       <c r="O22">
-        <v>488.1</v>
+        <v>100.03</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D23">
-        <v>243.69</v>
+        <v>102.9</v>
       </c>
       <c r="E23">
-        <v>276.88</v>
+        <v>104.8</v>
       </c>
       <c r="F23">
-        <v>318.74</v>
+        <v>105.06</v>
       </c>
       <c r="G23">
-        <v>377.97</v>
+        <v>109.5</v>
       </c>
       <c r="H23">
-        <v>379.81</v>
+        <v>110.3</v>
       </c>
       <c r="I23">
-        <v>415.04</v>
+        <v>107.9</v>
       </c>
       <c r="J23">
-        <v>519.83000000000004</v>
+        <v>111.4</v>
       </c>
       <c r="K23">
-        <v>489.22</v>
+        <v>110.58</v>
       </c>
       <c r="L23">
-        <v>526.72</v>
+        <v>100.9</v>
       </c>
       <c r="M23">
-        <v>503.48</v>
+        <v>95.5</v>
       </c>
       <c r="N23">
-        <v>456.47</v>
+        <v>95.6</v>
       </c>
       <c r="O23">
-        <v>343.9</v>
+        <v>99.8</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D24">
-        <v>22.771000000000001</v>
+        <v>4.3079999999999998</v>
       </c>
       <c r="E24">
-        <v>62.170999999999999</v>
+        <v>5.5030000000000001</v>
       </c>
       <c r="F24">
-        <v>86.138000000000005</v>
+        <v>6.3630000000000004</v>
       </c>
       <c r="G24">
-        <v>39.341000000000001</v>
+        <v>7.5720000000000001</v>
       </c>
       <c r="H24">
-        <v>43.756</v>
+        <v>6.4480000000000004</v>
       </c>
       <c r="I24">
-        <v>72.747</v>
+        <v>8.7129999999999992</v>
       </c>
       <c r="J24">
-        <v>68.355999999999995</v>
+        <v>10.923999999999999</v>
       </c>
       <c r="K24">
-        <v>114.628</v>
+        <v>11.342000000000001</v>
       </c>
       <c r="L24">
-        <v>127.676</v>
+        <v>10.234999999999999</v>
       </c>
       <c r="M24">
-        <v>155.512</v>
+        <v>7.3209999999999997</v>
       </c>
       <c r="N24">
-        <v>74.795000000000002</v>
+        <v>4.9509999999999996</v>
       </c>
       <c r="O24">
-        <v>49.411999999999999</v>
+        <v>5.1550000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D25">
-        <v>48.09</v>
+        <v>2231</v>
       </c>
       <c r="E25">
-        <v>40.591000000000001</v>
+        <v>1803</v>
       </c>
       <c r="F25">
-        <v>86.212000000000003</v>
+        <v>2214</v>
       </c>
       <c r="G25">
-        <v>66.989999999999995</v>
+        <v>2160</v>
       </c>
       <c r="H25">
-        <v>65.465000000000003</v>
+        <v>2070</v>
       </c>
       <c r="I25">
-        <v>56.097000000000001</v>
+        <v>2175</v>
       </c>
       <c r="J25">
-        <v>114.771</v>
+        <v>2504</v>
       </c>
       <c r="K25">
-        <v>99.522999999999996</v>
+        <v>2947</v>
       </c>
       <c r="L25">
-        <v>80.478999999999999</v>
+        <v>2879</v>
       </c>
       <c r="M25">
-        <v>101.77200000000001</v>
+        <v>2975</v>
       </c>
       <c r="N25">
-        <v>80.308999999999997</v>
+        <v>2431</v>
       </c>
       <c r="O25">
-        <v>71.730999999999995</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D26">
-        <v>597.41999999999996</v>
+        <v>8.1300000000000008</v>
       </c>
       <c r="E26">
-        <v>693.34</v>
+        <v>8.15</v>
       </c>
       <c r="F26">
-        <v>582.51</v>
+        <v>8.18</v>
       </c>
       <c r="G26">
-        <v>379.56</v>
+        <v>8.11</v>
       </c>
       <c r="H26">
-        <v>455.41</v>
+        <v>8.02</v>
       </c>
       <c r="I26">
-        <v>455.42</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="J26">
-        <v>495.98</v>
+        <v>8.02</v>
       </c>
       <c r="K26">
-        <v>594.41999999999996</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="L26">
-        <v>618.45000000000005</v>
+        <v>8.01</v>
       </c>
       <c r="M26">
-        <v>687.99</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="N26">
-        <v>655.97</v>
+        <v>8.02</v>
       </c>
       <c r="O26">
-        <v>660.34</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D27">
-        <v>413.32</v>
+        <v>8.14</v>
       </c>
       <c r="E27">
-        <v>441.52</v>
+        <v>8.15</v>
       </c>
       <c r="F27">
-        <v>439.51</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="G27">
-        <v>479.7</v>
+        <v>8.14</v>
       </c>
       <c r="H27">
-        <v>422.72</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="I27">
-        <v>399.74</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="J27">
-        <v>427.7</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="K27">
-        <v>394.84</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="L27">
-        <v>443.27</v>
+        <v>8.01</v>
       </c>
       <c r="M27">
-        <v>480.93</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="N27">
-        <v>514.62</v>
+        <v>8.02</v>
       </c>
       <c r="O27">
-        <v>489.59</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D28">
-        <v>735</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E28">
-        <v>578</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F28">
-        <v>736</v>
+        <v>0.107</v>
       </c>
       <c r="G28">
-        <v>639</v>
+        <v>0.127</v>
       </c>
       <c r="H28">
-        <v>1461</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="I28">
-        <v>1968</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J28">
-        <v>1796</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="K28">
-        <v>2151</v>
+        <v>0.08</v>
       </c>
       <c r="L28">
-        <v>2698</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="M28">
-        <v>2721</v>
+        <v>0.06</v>
       </c>
       <c r="N28">
-        <v>1575</v>
+        <v>6.2E-2</v>
       </c>
       <c r="O28">
-        <v>1470</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>18</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D29">
-        <v>835</v>
+        <v>2231</v>
       </c>
       <c r="E29">
-        <v>1349</v>
+        <v>1803</v>
       </c>
       <c r="F29">
-        <v>1734</v>
+        <v>2211</v>
       </c>
       <c r="G29">
-        <v>784</v>
+        <v>2160</v>
       </c>
       <c r="H29">
-        <v>1878</v>
+        <v>2166</v>
       </c>
       <c r="I29">
-        <v>1644</v>
+        <v>2176</v>
       </c>
       <c r="J29">
-        <v>1607</v>
+        <v>2503</v>
       </c>
       <c r="K29">
-        <v>1383</v>
+        <v>2859</v>
       </c>
       <c r="L29">
-        <v>1672</v>
+        <v>2879</v>
       </c>
       <c r="M29">
-        <v>2240</v>
+        <v>2975</v>
       </c>
       <c r="N29">
-        <v>2093</v>
+        <v>2431</v>
       </c>
       <c r="O29">
-        <v>2219</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D30">
-        <v>603.23</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="E30">
-        <v>684.37</v>
+        <v>8.06</v>
       </c>
       <c r="F30">
-        <v>619.19000000000005</v>
+        <v>8.08</v>
       </c>
       <c r="G30">
-        <v>383.01</v>
+        <v>8</v>
       </c>
       <c r="H30">
-        <v>451.42</v>
+        <v>7.9</v>
       </c>
       <c r="I30">
-        <v>460.3</v>
+        <v>7.92</v>
       </c>
       <c r="J30">
-        <v>494.31</v>
+        <v>7.89</v>
       </c>
       <c r="K30">
-        <v>584.83000000000004</v>
+        <v>7.91</v>
       </c>
       <c r="L30">
-        <v>606.46</v>
+        <v>7.89</v>
       </c>
       <c r="M30">
-        <v>657.86</v>
+        <v>7.91</v>
       </c>
       <c r="N30">
-        <v>649.95000000000005</v>
+        <v>7.91</v>
       </c>
       <c r="O30">
-        <v>660.58</v>
+        <v>7.99</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D31">
-        <v>409.79</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="E31">
-        <v>434.3</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="F31">
-        <v>454.31</v>
+        <v>8.11</v>
       </c>
       <c r="G31">
-        <v>493.13</v>
+        <v>8.0299999999999994</v>
       </c>
       <c r="H31">
-        <v>408.93</v>
+        <v>7.93</v>
       </c>
       <c r="I31">
-        <v>396</v>
+        <v>7.92</v>
       </c>
       <c r="J31">
-        <v>419.01</v>
+        <v>7.9</v>
       </c>
       <c r="K31">
-        <v>376.89</v>
+        <v>7.91</v>
       </c>
       <c r="L31">
-        <v>435.25</v>
+        <v>7.89</v>
       </c>
       <c r="M31">
-        <v>492.35</v>
+        <v>7.91</v>
       </c>
       <c r="N31">
-        <v>510.22</v>
+        <v>7.91</v>
       </c>
       <c r="O31">
-        <v>474.45</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
         <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D32">
-        <v>32.497</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E32">
-        <v>72.138000000000005</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="F32">
-        <v>123.81100000000001</v>
+        <v>0.107</v>
       </c>
       <c r="G32">
-        <v>55.793999999999997</v>
+        <v>0.128</v>
       </c>
       <c r="H32">
-        <v>49.122</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="I32">
-        <v>72.760000000000005</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J32">
-        <v>70.61</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K32">
-        <v>87.441999999999993</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="L32">
-        <v>108.318</v>
+        <v>0.06</v>
       </c>
       <c r="M32">
-        <v>138.864</v>
+        <v>0.06</v>
       </c>
       <c r="N32">
-        <v>49.804000000000002</v>
+        <v>6.3E-2</v>
       </c>
       <c r="O32">
-        <v>39.405999999999999</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D33">
-        <v>52.307000000000002</v>
+        <v>2231</v>
       </c>
       <c r="E33">
-        <v>71.436999999999998</v>
+        <v>1803</v>
       </c>
       <c r="F33">
-        <v>130.69900000000001</v>
+        <v>2210</v>
       </c>
       <c r="G33">
-        <v>84.088999999999999</v>
+        <v>2160</v>
       </c>
       <c r="H33">
-        <v>80.283000000000001</v>
+        <v>2166</v>
       </c>
       <c r="I33">
-        <v>60.74</v>
+        <v>2176</v>
       </c>
       <c r="J33">
-        <v>98.632999999999996</v>
+        <v>2503</v>
       </c>
       <c r="K33">
-        <v>85.686999999999998</v>
+        <v>2859</v>
       </c>
       <c r="L33">
-        <v>72.546000000000006</v>
+        <v>2878</v>
       </c>
       <c r="M33">
-        <v>90.863</v>
+        <v>2975</v>
       </c>
       <c r="N33">
-        <v>97.221000000000004</v>
+        <v>2431</v>
       </c>
       <c r="O33">
-        <v>90.843999999999994</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
         <v>27</v>
       </c>
-      <c r="B34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
       <c r="D34">
-        <v>8.01</v>
+        <v>30.59</v>
+      </c>
+      <c r="E34">
+        <v>30.62</v>
+      </c>
+      <c r="F34">
+        <v>30.28</v>
       </c>
       <c r="G34">
-        <v>8.17</v>
+        <v>29.14</v>
       </c>
       <c r="H34">
-        <v>8.1199999999999992</v>
+        <v>29.03</v>
       </c>
       <c r="I34">
-        <v>8.01</v>
+        <v>29.3</v>
       </c>
       <c r="J34">
-        <v>7.93</v>
+        <v>30.23</v>
       </c>
       <c r="K34">
-        <v>7.86</v>
+        <v>30.47</v>
       </c>
       <c r="L34">
-        <v>7.82</v>
+        <v>30.57</v>
       </c>
       <c r="M34">
-        <v>7.86</v>
+        <v>30.7</v>
       </c>
       <c r="N34">
-        <v>7.85</v>
+        <v>30.25</v>
       </c>
       <c r="O34">
-        <v>8.01</v>
+        <v>30.42</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
         <v>27</v>
       </c>
-      <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
       <c r="D35">
-        <v>8.1300000000000008</v>
+        <v>30.51</v>
       </c>
       <c r="E35">
-        <v>8.15</v>
+        <v>30.7</v>
       </c>
       <c r="F35">
-        <v>8.18</v>
+        <v>30.3</v>
       </c>
       <c r="G35">
-        <v>8.11</v>
+        <v>29.43</v>
       </c>
       <c r="H35">
-        <v>8.02</v>
+        <v>29.22</v>
       </c>
       <c r="I35">
-        <v>8.0399999999999991</v>
+        <v>29.24</v>
       </c>
       <c r="J35">
-        <v>8.02</v>
+        <v>30.23</v>
       </c>
       <c r="K35">
-        <v>8.0299999999999994</v>
+        <v>30.69</v>
       </c>
       <c r="L35">
-        <v>8.01</v>
+        <v>31.03</v>
       </c>
       <c r="M35">
-        <v>8.0299999999999994</v>
+        <v>31.03</v>
       </c>
       <c r="N35">
-        <v>8.02</v>
+        <v>30.09</v>
       </c>
       <c r="O35">
-        <v>8.1</v>
+        <v>30.51</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
         <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D36">
-        <v>449</v>
+        <v>1.087</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>0.74399999999999999</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="G36">
-        <v>249</v>
+        <v>1.474</v>
       </c>
       <c r="H36">
-        <v>1476</v>
+        <v>0.82</v>
       </c>
       <c r="I36">
-        <v>1763</v>
+        <v>0.66500000000000004</v>
       </c>
       <c r="J36">
-        <v>2210</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="K36">
-        <v>1838</v>
+        <v>0.77300000000000002</v>
       </c>
       <c r="L36">
-        <v>1680</v>
+        <v>1.0329999999999999</v>
       </c>
       <c r="M36">
-        <v>1850</v>
+        <v>0.997</v>
       </c>
       <c r="N36">
-        <v>753</v>
+        <v>0.86</v>
       </c>
       <c r="O36">
-        <v>561</v>
+        <v>0.81699999999999995</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D37">
         <v>2231</v>
@@ -2589,7 +2650,7 @@
         <v>1803</v>
       </c>
       <c r="F37">
-        <v>2211</v>
+        <v>2214</v>
       </c>
       <c r="G37">
         <v>2160</v>
@@ -2598,13 +2659,13 @@
         <v>2166</v>
       </c>
       <c r="I37">
-        <v>2158</v>
+        <v>2176</v>
       </c>
       <c r="J37">
-        <v>2503</v>
+        <v>2504</v>
       </c>
       <c r="K37">
-        <v>2859</v>
+        <v>2949</v>
       </c>
       <c r="L37">
         <v>2879</v>
@@ -2613,7 +2674,7 @@
         <v>2975</v>
       </c>
       <c r="N37">
-        <v>2421</v>
+        <v>2431</v>
       </c>
       <c r="O37">
         <v>2964</v>
@@ -2621,938 +2682,1643 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" t="s">
         <v>27</v>
       </c>
-      <c r="B38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" t="s">
-        <v>13</v>
-      </c>
       <c r="D38">
-        <v>8.01</v>
+        <v>1.38</v>
+      </c>
+      <c r="E38">
+        <v>1.33</v>
+      </c>
+      <c r="F38">
+        <v>2.6</v>
       </c>
       <c r="G38">
-        <v>8.15</v>
+        <v>5.83</v>
       </c>
       <c r="H38">
-        <v>8.11</v>
+        <v>9.84</v>
       </c>
       <c r="I38">
-        <v>8.02</v>
+        <v>13.42</v>
       </c>
       <c r="J38">
-        <v>7.93</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="K38">
-        <v>7.88</v>
+        <v>17.940000000000001</v>
       </c>
       <c r="L38">
-        <v>7.82</v>
+        <v>16.55</v>
       </c>
       <c r="M38">
-        <v>7.88</v>
+        <v>13.34</v>
       </c>
       <c r="N38">
-        <v>7.88</v>
+        <v>8.17</v>
       </c>
       <c r="O38">
-        <v>8.01</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" t="s">
         <v>27</v>
       </c>
-      <c r="B39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" t="s">
-        <v>13</v>
-      </c>
       <c r="D39">
-        <v>8.14</v>
+        <v>1.3</v>
       </c>
       <c r="E39">
-        <v>8.15</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F39">
-        <v>8.2100000000000009</v>
+        <v>2.74</v>
       </c>
       <c r="G39">
-        <v>8.14</v>
+        <v>5.56</v>
       </c>
       <c r="H39">
-        <v>8.0399999999999991</v>
+        <v>9.83</v>
       </c>
       <c r="I39">
-        <v>8.0399999999999991</v>
+        <v>13.37</v>
       </c>
       <c r="J39">
-        <v>8.0299999999999994</v>
+        <v>17.03</v>
       </c>
       <c r="K39">
-        <v>8.0399999999999991</v>
+        <v>17.91</v>
       </c>
       <c r="L39">
-        <v>8.01</v>
+        <v>16.45</v>
       </c>
       <c r="M39">
-        <v>8.0299999999999994</v>
+        <v>13.55</v>
       </c>
       <c r="N39">
-        <v>8.02</v>
+        <v>7.96</v>
       </c>
       <c r="O39">
-        <v>8.1</v>
+        <v>3.94</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
         <v>17</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D40">
-        <v>0.02</v>
+        <v>1.466</v>
+      </c>
+      <c r="E40">
+        <v>1.236</v>
+      </c>
+      <c r="F40">
+        <v>1.1830000000000001</v>
       </c>
       <c r="G40">
-        <v>4.2000000000000003E-2</v>
+        <v>1.4990000000000001</v>
       </c>
       <c r="H40">
-        <v>4.1000000000000002E-2</v>
+        <v>1.504</v>
       </c>
       <c r="I40">
-        <v>8.1000000000000003E-2</v>
+        <v>1.5429999999999999</v>
       </c>
       <c r="J40">
-        <v>5.1999999999999998E-2</v>
+        <v>1.56</v>
       </c>
       <c r="K40">
-        <v>0.08</v>
+        <v>1.35</v>
       </c>
       <c r="L40">
-        <v>7.0000000000000007E-2</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="M40">
-        <v>7.0999999999999994E-2</v>
+        <v>1.552</v>
       </c>
       <c r="N40">
-        <v>8.2000000000000003E-2</v>
+        <v>2.0779999999999998</v>
       </c>
       <c r="O40">
-        <v>2.5000000000000001E-2</v>
+        <v>1.5529999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D41">
-        <v>4.8000000000000001E-2</v>
+        <v>2231</v>
       </c>
       <c r="E41">
-        <v>6.4000000000000001E-2</v>
+        <v>1803</v>
       </c>
       <c r="F41">
-        <v>0.107</v>
+        <v>2214</v>
       </c>
       <c r="G41">
-        <v>0.127</v>
+        <v>2160</v>
       </c>
       <c r="H41">
-        <v>8.3000000000000004E-2</v>
+        <v>2166</v>
       </c>
       <c r="I41">
-        <v>7.0000000000000007E-2</v>
+        <v>2176</v>
       </c>
       <c r="J41">
-        <v>7.5999999999999998E-2</v>
+        <v>2504</v>
       </c>
       <c r="K41">
-        <v>0.08</v>
+        <v>2949</v>
       </c>
       <c r="L41">
-        <v>6.0999999999999999E-2</v>
+        <v>2879</v>
       </c>
       <c r="M41">
-        <v>0.06</v>
+        <v>2975</v>
       </c>
       <c r="N41">
-        <v>6.2E-2</v>
+        <v>2894</v>
       </c>
       <c r="O41">
-        <v>0.05</v>
+        <v>2975</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C42" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D42">
-        <v>29.02</v>
+        <v>376.17</v>
       </c>
       <c r="E42">
-        <v>28.55</v>
+        <v>473.45</v>
       </c>
       <c r="F42">
-        <v>27.53</v>
+        <v>407.76</v>
       </c>
       <c r="G42">
-        <v>26.38</v>
+        <v>301.83999999999997</v>
       </c>
       <c r="H42">
-        <v>28.32</v>
+        <v>398.42</v>
       </c>
       <c r="I42">
-        <v>29.38</v>
+        <v>464.58</v>
       </c>
       <c r="J42">
-        <v>29.77</v>
+        <v>566.19000000000005</v>
       </c>
       <c r="K42">
-        <v>29.93</v>
+        <v>723.6</v>
       </c>
       <c r="L42">
-        <v>30.26</v>
+        <v>736.16</v>
       </c>
       <c r="M42">
-        <v>30.25</v>
+        <v>729.35</v>
       </c>
       <c r="N42">
-        <v>28.94</v>
+        <v>576.75</v>
       </c>
       <c r="O42">
-        <v>27.79</v>
+        <v>491.44</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D43">
-        <v>30.59</v>
+        <v>378.6</v>
       </c>
       <c r="E43">
-        <v>30.62</v>
+        <v>464</v>
       </c>
       <c r="F43">
-        <v>30.28</v>
+        <v>431.3</v>
       </c>
       <c r="G43">
-        <v>29.14</v>
+        <v>304.8</v>
       </c>
       <c r="H43">
-        <v>29.03</v>
+        <v>392.4</v>
       </c>
       <c r="I43">
-        <v>29.31</v>
+        <v>467.55</v>
       </c>
       <c r="J43">
-        <v>30.23</v>
+        <v>565.83000000000004</v>
       </c>
       <c r="K43">
-        <v>30.47</v>
+        <v>714.12</v>
       </c>
       <c r="L43">
-        <v>30.57</v>
+        <v>704.93</v>
       </c>
       <c r="M43">
-        <v>30.7</v>
+        <v>707.4</v>
       </c>
       <c r="N43">
-        <v>30.26</v>
+        <v>562.75</v>
       </c>
       <c r="O43">
-        <v>30.42</v>
+        <v>488.1</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
         <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D44">
-        <v>1193</v>
+        <v>22.771000000000001</v>
       </c>
       <c r="E44">
-        <v>670</v>
+        <v>62.170999999999999</v>
       </c>
       <c r="F44">
-        <v>744</v>
+        <v>86.138000000000005</v>
       </c>
       <c r="G44">
-        <v>721</v>
+        <v>39.341000000000001</v>
       </c>
       <c r="H44">
-        <v>2220</v>
+        <v>43.756</v>
       </c>
       <c r="I44">
-        <v>2829</v>
+        <v>72.747</v>
       </c>
       <c r="J44">
-        <v>2836</v>
+        <v>68.355999999999995</v>
       </c>
       <c r="K44">
-        <v>2964</v>
+        <v>114.628</v>
       </c>
       <c r="L44">
-        <v>2122</v>
+        <v>127.676</v>
       </c>
       <c r="M44">
-        <v>2873</v>
+        <v>155.512</v>
       </c>
       <c r="N44">
-        <v>2306</v>
+        <v>74.795000000000002</v>
       </c>
       <c r="O44">
-        <v>2229</v>
+        <v>49.411999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
       </c>
       <c r="C45" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D45">
-        <v>2231</v>
+        <v>735</v>
       </c>
       <c r="E45">
-        <v>1803</v>
+        <v>578</v>
       </c>
       <c r="F45">
-        <v>2214</v>
+        <v>736</v>
       </c>
       <c r="G45">
-        <v>2160</v>
+        <v>639</v>
       </c>
       <c r="H45">
-        <v>2166</v>
+        <v>1461</v>
       </c>
       <c r="I45">
-        <v>2158</v>
+        <v>1968</v>
       </c>
       <c r="J45">
-        <v>2504</v>
+        <v>1802</v>
       </c>
       <c r="K45">
-        <v>2949</v>
+        <v>2151</v>
       </c>
       <c r="L45">
-        <v>2879</v>
+        <v>2699</v>
       </c>
       <c r="M45">
-        <v>2975</v>
+        <v>2721</v>
       </c>
       <c r="N45">
-        <v>2421</v>
+        <v>1575</v>
       </c>
       <c r="O45">
-        <v>2964</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D46">
-        <v>29.35</v>
+        <v>597.41999999999996</v>
       </c>
       <c r="E46">
-        <v>28.79</v>
+        <v>693.34</v>
       </c>
       <c r="F46">
-        <v>27.78</v>
+        <v>582.51</v>
       </c>
       <c r="G46">
-        <v>27.3</v>
+        <v>379.56</v>
       </c>
       <c r="H46">
-        <v>28.69</v>
+        <v>455.41</v>
       </c>
       <c r="I46">
-        <v>29.67</v>
+        <v>455.42</v>
       </c>
       <c r="J46">
-        <v>29.91</v>
+        <v>495.98</v>
       </c>
       <c r="K46">
-        <v>30.01</v>
+        <v>594.41999999999996</v>
       </c>
       <c r="L46">
-        <v>30.34</v>
+        <v>618.45000000000005</v>
       </c>
       <c r="M46">
-        <v>30.47</v>
+        <v>687.99</v>
       </c>
       <c r="N46">
-        <v>29.63</v>
+        <v>655.97</v>
       </c>
       <c r="O46">
-        <v>29.67</v>
+        <v>660.34</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D47">
-        <v>30.51</v>
+        <v>603.23</v>
       </c>
       <c r="E47">
-        <v>30.7</v>
+        <v>684.37</v>
       </c>
       <c r="F47">
-        <v>30.3</v>
+        <v>619.19000000000005</v>
       </c>
       <c r="G47">
-        <v>29.43</v>
+        <v>383.01</v>
       </c>
       <c r="H47">
-        <v>29.22</v>
+        <v>451.42</v>
       </c>
       <c r="I47">
-        <v>29.26</v>
+        <v>460.3</v>
       </c>
       <c r="J47">
-        <v>30.23</v>
+        <v>494.31</v>
       </c>
       <c r="K47">
-        <v>30.69</v>
+        <v>584.83000000000004</v>
       </c>
       <c r="L47">
-        <v>31.03</v>
+        <v>606.46</v>
       </c>
       <c r="M47">
-        <v>31.03</v>
+        <v>657.86</v>
       </c>
       <c r="N47">
-        <v>30.09</v>
+        <v>649.95000000000005</v>
       </c>
       <c r="O47">
-        <v>30.51</v>
+        <v>660.58</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D48">
-        <v>1.345</v>
+        <v>32.497</v>
       </c>
       <c r="E48">
-        <v>1.2869999999999999</v>
+        <v>72.138000000000005</v>
       </c>
       <c r="F48">
-        <v>1.07</v>
+        <v>123.81100000000001</v>
       </c>
       <c r="G48">
-        <v>2.8039999999999998</v>
+        <v>55.793999999999997</v>
       </c>
       <c r="H48">
-        <v>1.972</v>
+        <v>49.122</v>
       </c>
       <c r="I48">
-        <v>1.3129999999999999</v>
+        <v>72.760000000000005</v>
       </c>
       <c r="J48">
-        <v>0.85799999999999998</v>
+        <v>70.61</v>
       </c>
       <c r="K48">
-        <v>0.79400000000000004</v>
+        <v>87.441999999999993</v>
       </c>
       <c r="L48">
-        <v>0.90800000000000003</v>
+        <v>108.318</v>
       </c>
       <c r="M48">
-        <v>1.163</v>
+        <v>138.864</v>
       </c>
       <c r="N48">
-        <v>2.0070000000000001</v>
+        <v>49.804000000000002</v>
       </c>
       <c r="O48">
-        <v>4.0190000000000001</v>
+        <v>39.405999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
       </c>
       <c r="C49" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D49">
-        <v>1.087</v>
+        <v>735</v>
       </c>
       <c r="E49">
-        <v>0.74399999999999999</v>
+        <v>578</v>
       </c>
       <c r="F49">
-        <v>0.59299999999999997</v>
+        <v>736</v>
       </c>
       <c r="G49">
-        <v>1.474</v>
+        <v>639</v>
       </c>
       <c r="H49">
-        <v>0.82</v>
+        <v>1461</v>
       </c>
       <c r="I49">
-        <v>0.66500000000000004</v>
+        <v>1968</v>
       </c>
       <c r="J49">
-        <v>0.79500000000000004</v>
+        <v>1796</v>
       </c>
       <c r="K49">
-        <v>0.77300000000000002</v>
+        <v>2151</v>
       </c>
       <c r="L49">
-        <v>1.0329999999999999</v>
+        <v>2698</v>
       </c>
       <c r="M49">
-        <v>0.997</v>
+        <v>2721</v>
       </c>
       <c r="N49">
-        <v>0.85899999999999999</v>
+        <v>1575</v>
       </c>
       <c r="O49">
-        <v>0.81699999999999995</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D50">
-        <v>2.54</v>
+        <v>405.84</v>
       </c>
       <c r="E50">
-        <v>2.91</v>
+        <v>399.88</v>
       </c>
       <c r="F50">
-        <v>3.58</v>
+        <v>401.33</v>
       </c>
       <c r="G50">
-        <v>6.68</v>
+        <v>402.06</v>
       </c>
       <c r="H50">
-        <v>9.2100000000000009</v>
+        <v>378.21</v>
       </c>
       <c r="I50">
-        <v>12.71</v>
+        <v>345.81</v>
       </c>
       <c r="J50">
-        <v>15.49</v>
+        <v>331.59</v>
       </c>
       <c r="K50">
-        <v>16.88</v>
+        <v>305.08999999999997</v>
       </c>
       <c r="L50">
-        <v>16.22</v>
+        <v>284.74</v>
       </c>
       <c r="M50">
-        <v>13.17</v>
+        <v>289.47000000000003</v>
       </c>
       <c r="N50">
-        <v>9.0399999999999991</v>
+        <v>313.97000000000003</v>
       </c>
       <c r="O50">
-        <v>5.7</v>
+        <v>344.18</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B51" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D51">
-        <v>1.38</v>
+        <v>406.86</v>
       </c>
       <c r="E51">
-        <v>1.33</v>
+        <v>400.02</v>
       </c>
       <c r="F51">
-        <v>2.6</v>
+        <v>401.79</v>
       </c>
       <c r="G51">
-        <v>5.83</v>
+        <v>404.42</v>
       </c>
       <c r="H51">
-        <v>9.84</v>
+        <v>377.87</v>
       </c>
       <c r="I51">
-        <v>13.43</v>
+        <v>347.11</v>
       </c>
       <c r="J51">
-        <v>17.100000000000001</v>
+        <v>329.22</v>
       </c>
       <c r="K51">
-        <v>17.940000000000001</v>
+        <v>310.06</v>
       </c>
       <c r="L51">
-        <v>16.55</v>
+        <v>292.24</v>
       </c>
       <c r="M51">
-        <v>13.34</v>
+        <v>300.29000000000002</v>
       </c>
       <c r="N51">
-        <v>8.16</v>
+        <v>315.06</v>
       </c>
       <c r="O51">
-        <v>4.08</v>
+        <v>338.6</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B52" t="s">
         <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D52">
-        <v>1193</v>
+        <v>3.5649999999999999</v>
       </c>
       <c r="E52">
-        <v>670</v>
+        <v>6.2539999999999996</v>
       </c>
       <c r="F52">
-        <v>744</v>
+        <v>4.9859999999999998</v>
       </c>
       <c r="G52">
-        <v>726</v>
+        <v>11.957000000000001</v>
       </c>
       <c r="H52">
-        <v>2220</v>
+        <v>18.794</v>
       </c>
       <c r="I52">
-        <v>2829</v>
+        <v>20.538</v>
       </c>
       <c r="J52">
-        <v>2888</v>
+        <v>24.295999999999999</v>
       </c>
       <c r="K52">
-        <v>2968</v>
+        <v>27.3</v>
       </c>
       <c r="L52">
-        <v>2867</v>
+        <v>37.084000000000003</v>
       </c>
       <c r="M52">
-        <v>2969</v>
+        <v>32.222000000000001</v>
       </c>
       <c r="N52">
-        <v>2313</v>
+        <v>16.943999999999999</v>
       </c>
       <c r="O52">
-        <v>2232</v>
+        <v>26.562000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B53" t="s">
         <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D53">
-        <v>2231</v>
+        <v>175</v>
       </c>
       <c r="E53">
-        <v>1803</v>
+        <v>534</v>
       </c>
       <c r="F53">
-        <v>2214</v>
+        <v>376</v>
       </c>
       <c r="G53">
-        <v>2160</v>
+        <v>687</v>
       </c>
       <c r="H53">
-        <v>2166</v>
+        <v>2218</v>
       </c>
       <c r="I53">
-        <v>2158</v>
+        <v>2072</v>
       </c>
       <c r="J53">
-        <v>2504</v>
+        <v>1464</v>
       </c>
       <c r="K53">
-        <v>2949</v>
+        <v>2161</v>
       </c>
       <c r="L53">
-        <v>2879</v>
+        <v>2732</v>
       </c>
       <c r="M53">
-        <v>2975</v>
+        <v>2660</v>
       </c>
       <c r="N53">
-        <v>2884</v>
+        <v>1975</v>
       </c>
       <c r="O53">
-        <v>2975</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D54">
-        <v>1.63</v>
+        <v>13.34</v>
       </c>
       <c r="E54">
-        <v>2.8</v>
+        <v>13.14</v>
       </c>
       <c r="F54">
-        <v>3.52</v>
+        <v>13.19</v>
       </c>
       <c r="G54">
-        <v>6.82</v>
+        <v>13.21</v>
       </c>
       <c r="H54">
-        <v>9.2799999999999994</v>
+        <v>12.43</v>
       </c>
       <c r="I54">
-        <v>12.79</v>
+        <v>11.36</v>
       </c>
       <c r="J54">
-        <v>15.6</v>
+        <v>10.9</v>
       </c>
       <c r="K54">
-        <v>16.850000000000001</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="L54">
-        <v>16.260000000000002</v>
+        <v>9.36</v>
       </c>
       <c r="M54">
-        <v>13.48</v>
+        <v>9.51</v>
       </c>
       <c r="N54">
-        <v>8.9499999999999993</v>
+        <v>10.32</v>
       </c>
       <c r="O54">
-        <v>5.79</v>
+        <v>11.31</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D55">
-        <v>1.3</v>
+        <v>13.37</v>
       </c>
       <c r="E55">
-        <v>1.1000000000000001</v>
+        <v>13.15</v>
       </c>
       <c r="F55">
-        <v>2.74</v>
+        <v>13.2</v>
       </c>
       <c r="G55">
-        <v>5.56</v>
+        <v>13.29</v>
       </c>
       <c r="H55">
-        <v>9.83</v>
+        <v>12.42</v>
       </c>
       <c r="I55">
-        <v>13.4</v>
+        <v>11.41</v>
       </c>
       <c r="J55">
-        <v>17.03</v>
+        <v>10.82</v>
       </c>
       <c r="K55">
-        <v>17.91</v>
+        <v>10.19</v>
       </c>
       <c r="L55">
-        <v>16.45</v>
+        <v>9.6</v>
       </c>
       <c r="M55">
-        <v>13.55</v>
+        <v>9.8699999999999992</v>
       </c>
       <c r="N55">
-        <v>7.95</v>
+        <v>10.35</v>
       </c>
       <c r="O55">
-        <v>3.94</v>
+        <v>11.13</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
         <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D56">
-        <v>2.06</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="E56">
-        <v>0.76</v>
+        <v>0.20599999999999999</v>
       </c>
       <c r="F56">
-        <v>0.502</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="G56">
-        <v>0.872</v>
+        <v>0.39300000000000002</v>
       </c>
       <c r="H56">
-        <v>1.343</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="I56">
-        <v>1.3049999999999999</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="J56">
-        <v>1.375</v>
+        <v>0.79800000000000004</v>
       </c>
       <c r="K56">
-        <v>1.17</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="L56">
-        <v>1.139</v>
+        <v>1.2190000000000001</v>
       </c>
       <c r="M56">
-        <v>1.5509999999999999</v>
+        <v>1.0589999999999999</v>
       </c>
       <c r="N56">
-        <v>1.629</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="O56">
-        <v>1.754</v>
+        <v>0.873</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
         <v>18</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D57">
-        <v>1.466</v>
+        <v>175</v>
       </c>
       <c r="E57">
-        <v>1.236</v>
+        <v>534</v>
       </c>
       <c r="F57">
-        <v>1.1830000000000001</v>
+        <v>376</v>
       </c>
       <c r="G57">
-        <v>1.4990000000000001</v>
+        <v>687</v>
       </c>
       <c r="H57">
-        <v>1.504</v>
+        <v>2218</v>
       </c>
       <c r="I57">
-        <v>1.544</v>
+        <v>2072</v>
       </c>
       <c r="J57">
-        <v>1.56</v>
+        <v>1464</v>
       </c>
       <c r="K57">
-        <v>1.35</v>
+        <v>2161</v>
       </c>
       <c r="L57">
-        <v>1.2969999999999999</v>
+        <v>2732</v>
       </c>
       <c r="M57">
-        <v>1.552</v>
+        <v>2660</v>
       </c>
       <c r="N57">
-        <v>2.0779999999999998</v>
+        <v>1975</v>
       </c>
       <c r="O57">
-        <v>1.5529999999999999</v>
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G58">
+        <v>1.91</v>
+      </c>
+      <c r="H58">
+        <v>1.99</v>
+      </c>
+      <c r="I58">
+        <v>1.61</v>
+      </c>
+      <c r="J58">
+        <v>1.76</v>
+      </c>
+      <c r="K58">
+        <v>1.71</v>
+      </c>
+      <c r="L58">
+        <v>1.51</v>
+      </c>
+      <c r="M58">
+        <v>1.64</v>
+      </c>
+      <c r="N58">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+      <c r="G59">
+        <v>1.91</v>
+      </c>
+      <c r="H59">
+        <v>1.97</v>
+      </c>
+      <c r="I59">
+        <v>1.67</v>
+      </c>
+      <c r="J59">
+        <v>1.83</v>
+      </c>
+      <c r="K59">
+        <v>1.79</v>
+      </c>
+      <c r="L59">
+        <v>1.44</v>
+      </c>
+      <c r="M59">
+        <v>1.61</v>
+      </c>
+      <c r="N59">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60">
+        <v>9.4E-2</v>
+      </c>
+      <c r="H60">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="I60">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="J60">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K60">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="L60">
+        <v>0.37</v>
+      </c>
+      <c r="M60">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N60">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>174</v>
+      </c>
+      <c r="H61">
+        <v>725</v>
+      </c>
+      <c r="I61">
+        <v>1030</v>
+      </c>
+      <c r="J61">
+        <v>1322</v>
+      </c>
+      <c r="K61">
+        <v>1112</v>
+      </c>
+      <c r="L61">
+        <v>1047</v>
+      </c>
+      <c r="M61">
+        <v>1542</v>
+      </c>
+      <c r="N61">
+        <v>158</v>
+      </c>
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62">
+        <v>8.01</v>
+      </c>
+      <c r="G62">
+        <v>8.17</v>
+      </c>
+      <c r="H62">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="I62">
+        <v>8.01</v>
+      </c>
+      <c r="J62">
+        <v>7.93</v>
+      </c>
+      <c r="K62">
+        <v>7.86</v>
+      </c>
+      <c r="L62">
+        <v>7.82</v>
+      </c>
+      <c r="M62">
+        <v>7.86</v>
+      </c>
+      <c r="N62">
+        <v>7.85</v>
+      </c>
+      <c r="O62">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63">
+        <v>8.01</v>
+      </c>
+      <c r="G63">
+        <v>8.15</v>
+      </c>
+      <c r="H63">
+        <v>8.11</v>
+      </c>
+      <c r="I63">
+        <v>8.02</v>
+      </c>
+      <c r="J63">
+        <v>7.93</v>
+      </c>
+      <c r="K63">
+        <v>7.88</v>
+      </c>
+      <c r="L63">
+        <v>7.82</v>
+      </c>
+      <c r="M63">
+        <v>7.88</v>
+      </c>
+      <c r="N63">
+        <v>7.88</v>
+      </c>
+      <c r="O63">
+        <v>8.01</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64">
+        <v>0.02</v>
+      </c>
+      <c r="G64">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H64">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="I64">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="J64">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K64">
+        <v>0.08</v>
+      </c>
+      <c r="L64">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M64">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="N64">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O64">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65">
+        <v>449</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>249</v>
+      </c>
+      <c r="H65">
+        <v>1476</v>
+      </c>
+      <c r="I65">
+        <v>1763</v>
+      </c>
+      <c r="J65">
+        <v>2210</v>
+      </c>
+      <c r="K65">
+        <v>1838</v>
+      </c>
+      <c r="L65">
+        <v>1680</v>
+      </c>
+      <c r="M65">
+        <v>1850</v>
+      </c>
+      <c r="N65">
+        <v>753</v>
+      </c>
+      <c r="O65">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>32</v>
+      </c>
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66">
+        <v>29.02</v>
+      </c>
+      <c r="E66">
+        <v>28.55</v>
+      </c>
+      <c r="F66">
+        <v>27.53</v>
+      </c>
+      <c r="G66">
+        <v>26.38</v>
+      </c>
+      <c r="H66">
+        <v>28.32</v>
+      </c>
+      <c r="I66">
+        <v>29.38</v>
+      </c>
+      <c r="J66">
+        <v>29.77</v>
+      </c>
+      <c r="K66">
+        <v>29.93</v>
+      </c>
+      <c r="L66">
+        <v>30.26</v>
+      </c>
+      <c r="M66">
+        <v>30.25</v>
+      </c>
+      <c r="N66">
+        <v>28.94</v>
+      </c>
+      <c r="O66">
+        <v>27.79</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" t="s">
+        <v>34</v>
+      </c>
+      <c r="D67">
+        <v>29.35</v>
+      </c>
+      <c r="E67">
+        <v>28.79</v>
+      </c>
+      <c r="F67">
+        <v>27.78</v>
+      </c>
+      <c r="G67">
+        <v>27.3</v>
+      </c>
+      <c r="H67">
+        <v>28.69</v>
+      </c>
+      <c r="I67">
+        <v>29.67</v>
+      </c>
+      <c r="J67">
+        <v>29.91</v>
+      </c>
+      <c r="K67">
+        <v>30.01</v>
+      </c>
+      <c r="L67">
+        <v>30.34</v>
+      </c>
+      <c r="M67">
+        <v>30.47</v>
+      </c>
+      <c r="N67">
+        <v>29.63</v>
+      </c>
+      <c r="O67">
+        <v>29.67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>34</v>
+      </c>
+      <c r="D68">
+        <v>1.345</v>
+      </c>
+      <c r="E68">
+        <v>1.2869999999999999</v>
+      </c>
+      <c r="F68">
+        <v>1.07</v>
+      </c>
+      <c r="G68">
+        <v>2.8039999999999998</v>
+      </c>
+      <c r="H68">
+        <v>1.972</v>
+      </c>
+      <c r="I68">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="J68">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="K68">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="L68">
+        <v>0.90800000000000003</v>
+      </c>
+      <c r="M68">
+        <v>1.163</v>
+      </c>
+      <c r="N68">
+        <v>2.0070000000000001</v>
+      </c>
+      <c r="O68">
+        <v>4.0190000000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69">
+        <v>1193</v>
+      </c>
+      <c r="E69">
+        <v>670</v>
+      </c>
+      <c r="F69">
+        <v>744</v>
+      </c>
+      <c r="G69">
+        <v>721</v>
+      </c>
+      <c r="H69">
+        <v>2220</v>
+      </c>
+      <c r="I69">
+        <v>2829</v>
+      </c>
+      <c r="J69">
+        <v>2836</v>
+      </c>
+      <c r="K69">
+        <v>2964</v>
+      </c>
+      <c r="L69">
+        <v>2122</v>
+      </c>
+      <c r="M69">
+        <v>2873</v>
+      </c>
+      <c r="N69">
+        <v>2306</v>
+      </c>
+      <c r="O69">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="s">
+        <v>34</v>
+      </c>
+      <c r="D70">
+        <v>2.54</v>
+      </c>
+      <c r="E70">
+        <v>2.91</v>
+      </c>
+      <c r="F70">
+        <v>3.58</v>
+      </c>
+      <c r="G70">
+        <v>6.68</v>
+      </c>
+      <c r="H70">
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="I70">
+        <v>12.71</v>
+      </c>
+      <c r="J70">
+        <v>15.49</v>
+      </c>
+      <c r="K70">
+        <v>16.88</v>
+      </c>
+      <c r="L70">
+        <v>16.22</v>
+      </c>
+      <c r="M70">
+        <v>13.17</v>
+      </c>
+      <c r="N70">
+        <v>9.0399999999999991</v>
+      </c>
+      <c r="O70">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>33</v>
+      </c>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" t="s">
+        <v>34</v>
+      </c>
+      <c r="D71">
+        <v>1.63</v>
+      </c>
+      <c r="E71">
+        <v>2.8</v>
+      </c>
+      <c r="F71">
+        <v>3.52</v>
+      </c>
+      <c r="G71">
+        <v>6.82</v>
+      </c>
+      <c r="H71">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="I71">
+        <v>12.79</v>
+      </c>
+      <c r="J71">
+        <v>15.6</v>
+      </c>
+      <c r="K71">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="L71">
+        <v>16.260000000000002</v>
+      </c>
+      <c r="M71">
+        <v>13.48</v>
+      </c>
+      <c r="N71">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="O71">
+        <v>5.79</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>33</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72" t="s">
+        <v>34</v>
+      </c>
+      <c r="D72">
+        <v>2.06</v>
+      </c>
+      <c r="E72">
+        <v>0.76</v>
+      </c>
+      <c r="F72">
+        <v>0.502</v>
+      </c>
+      <c r="G72">
+        <v>0.872</v>
+      </c>
+      <c r="H72">
+        <v>1.343</v>
+      </c>
+      <c r="I72">
+        <v>1.3049999999999999</v>
+      </c>
+      <c r="J72">
+        <v>1.375</v>
+      </c>
+      <c r="K72">
+        <v>1.17</v>
+      </c>
+      <c r="L72">
+        <v>1.139</v>
+      </c>
+      <c r="M72">
+        <v>1.5509999999999999</v>
+      </c>
+      <c r="N72">
+        <v>1.629</v>
+      </c>
+      <c r="O72">
+        <v>1.754</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>33</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" t="s">
+        <v>34</v>
+      </c>
+      <c r="D73">
+        <v>1193</v>
+      </c>
+      <c r="E73">
+        <v>670</v>
+      </c>
+      <c r="F73">
+        <v>744</v>
+      </c>
+      <c r="G73">
+        <v>726</v>
+      </c>
+      <c r="H73">
+        <v>2220</v>
+      </c>
+      <c r="I73">
+        <v>2829</v>
+      </c>
+      <c r="J73">
+        <v>2888</v>
+      </c>
+      <c r="K73">
+        <v>2968</v>
+      </c>
+      <c r="L73">
+        <v>2867</v>
+      </c>
+      <c r="M73">
+        <v>2969</v>
+      </c>
+      <c r="N73">
+        <v>2313</v>
+      </c>
+      <c r="O73">
+        <v>2232</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:O57">
-    <sortCondition ref="A2:A57"/>
-    <sortCondition ref="C2:C57"/>
-    <sortCondition ref="B2:B57"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>